<commit_message>
Grunt, Maps experiments, google maps api test
</commit_message>
<xml_diff>
--- a/Data/Migration Statistics 2012 optimized.xlsx
+++ b/Data/Migration Statistics 2012 optimized.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="27200" windowHeight="14820" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="14580" yWindow="13520" windowWidth="27200" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="OECD.Stat export" sheetId="1" r:id="rId1"/>
@@ -1224,8 +1224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HG42"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:HG42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F3" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -69335,8 +69335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HF34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Z25" sqref="Z25"/>
+    <sheetView topLeftCell="EK1" workbookViewId="0">
+      <selection activeCell="ES11" sqref="ES11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -91239,6 +91239,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:GZ34">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:GZ11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>